<commit_message>
Updated to add a checkpoint to verify that the candidate was properly created, a highlight of the Recruiting menu item before clicking on it to allow the app to catch up to the script, and statement to add the dynamically created name to the datasheet value, so that the checkpoint will look for the dynamic values, and the OR properties of the checkpoint object will use that value too.
</commit_message>
<xml_diff>
--- a/SAP_Success_Factors_AI/Default.xlsx
+++ b/SAP_Success_Factors_AI/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>United States</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>partRioDC8</t>
+  </si>
+  <si>
+    <t>FullName</t>
   </si>
   <si>
     <t>URL</t>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -549,12 +552,13 @@
     <col min="4" max="4" width="15.75390625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.10546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.97265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.41796875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c t="s">
         <v>2</v>
@@ -563,13 +567,16 @@
         <v>6</v>
       </c>
       <c t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c t="s">
         <v>1</v>
       </c>
       <c t="s">
         <v>5</v>
+      </c>
+      <c t="s">
+        <v>9</v>
       </c>
     </row>
     <row>
@@ -588,9 +595,10 @@
       <c s="1">
         <v>1234567890</v>
       </c>
-      <c s="3" t="s">
+      <c s="1" t="s">
         <v>0</v>
       </c>
+      <c s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>